<commit_message>
Birthday commit! Set values as displayed for all excel sheets.
</commit_message>
<xml_diff>
--- a/test_files/MSE_tests/dHAP4_15_gene_network_deletion_added_input_KD_20160126.xlsx
+++ b/test_files/MSE_tests/dHAP4_15_gene_network_deletion_added_input_KD_20160126.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <workbookPr date1904="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\GRNmap\Troubleshooting_20150112\2016-01-26\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GRNmap\test_files\MSE_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="360" windowWidth="20565" windowHeight="14640" tabRatio="858" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="2025" yWindow="360" windowWidth="20565" windowHeight="14640" tabRatio="858" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="optimization_parameters" sheetId="10" r:id="rId10"/>
     <sheet name="threshold_b" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511" fullPrecision="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -510,6 +510,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -545,6 +562,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -720,19 +754,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,184 +774,184 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="10">
-        <v>0.46209820000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.46210000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="10">
-        <v>0.69314719999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.69310000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>5.436448E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.4399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="10">
-        <v>5.436448E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.4399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>0.46209820000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.46210000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10">
-        <v>5.436448E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.4399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="10">
-        <v>5.4364483999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.4399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="10">
-        <v>0.69314719999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.69310000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="10">
-        <v>9.2419619999999994E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.2399999999999996E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="10">
-        <v>3.7467420000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="10">
-        <v>9.8318740000000009E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.7999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="10">
-        <v>5.436448E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.4399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="10">
-        <v>0.46209820000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.46210000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="10">
-        <v>0.46209820000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.46210000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="10">
-        <v>8.5048740000000008E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
     </row>
   </sheetData>
@@ -932,19 +966,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -952,7 +986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -960,7 +994,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -968,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -976,7 +1010,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -984,7 +1018,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -992,7 +1026,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1000,7 +1034,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1008,7 +1042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1016,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1024,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1032,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1040,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1048,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1062,7 +1096,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1082,7 +1116,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1137,19 +1171,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1173,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1181,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1189,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1197,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1221,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1229,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1237,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1245,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1253,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1261,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1269,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1277,40 +1311,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
     </row>
   </sheetData>
@@ -1328,19 +1362,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1348,181 +1382,181 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="9">
-        <v>0.23104910000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="9">
-        <v>0.34657359999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.34660000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
-        <v>2.718224E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.7199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="9">
-        <v>2.718224E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.7199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="9">
-        <v>0.23104910000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="9">
-        <v>2.718224E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.7199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="11">
-        <v>2.7182241999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.7199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="9">
-        <v>0.34657359999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.34660000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="8">
-        <v>4.6209809999999997E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.6199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="8">
-        <v>1.8733710000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.8700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="9">
-        <v>4.9159370000000004E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="9">
-        <v>2.718224E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.7199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="9">
-        <v>0.23104910000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="9">
-        <v>0.23104910000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="9">
-        <v>4.2524370000000004E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4.3E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
     </row>
   </sheetData>
@@ -1536,16 +1570,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1609,7 +1643,7 @@
         <v>0.5827</v>
       </c>
       <c r="G2" s="14">
-        <v>-2.5174999999999989E-2</v>
+        <v>-2.52E-2</v>
       </c>
       <c r="H2" s="7">
         <v>-0.3947</v>
@@ -1633,7 +1667,7 @@
         <v>-1.2497</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1677,7 +1711,7 @@
         <v>-0.92479999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1721,7 +1755,7 @@
         <v>1.4784999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1765,7 +1799,7 @@
         <v>-0.35849999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1809,7 +1843,7 @@
         <v>0.1953</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1853,7 +1887,7 @@
         <v>-1.8463000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1897,7 +1931,7 @@
         <v>2.2172000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1941,7 +1975,7 @@
         <v>-0.12709999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1985,7 +2019,7 @@
         <v>-1.0367</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2029,7 +2063,7 @@
         <v>-0.27479999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2073,7 +2107,7 @@
         <v>0.28120000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2117,7 +2151,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2161,7 +2195,7 @@
         <v>-0.72499999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2205,7 +2239,7 @@
         <v>-0.51170000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -2246,10 +2280,10 @@
         <v>1.3863000000000001</v>
       </c>
       <c r="N16" s="12">
-        <v>2.6346000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.6345999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2265,7 +2299,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2281,7 +2315,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2297,7 +2331,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2312,7 +2346,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2328,7 +2362,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2344,7 +2378,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2360,7 +2394,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2375,7 +2409,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2391,7 +2425,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2422,16 +2456,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2472,7 +2506,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2498,7 +2532,7 @@
         <v>-0.42530000000000001</v>
       </c>
       <c r="I2" s="13">
-        <v>-0.17026666666666668</v>
+        <v>-0.17030000000000001</v>
       </c>
       <c r="J2" s="10">
         <v>0.56820000000000004</v>
@@ -2513,7 +2547,7 @@
         <v>-0.38879999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2554,7 +2588,7 @@
         <v>-1.3284</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2583,7 +2617,7 @@
         <v>0.59750000000000003</v>
       </c>
       <c r="J4" s="13">
-        <v>7.8900000000000012E-2</v>
+        <v>7.8899999999999998E-2</v>
       </c>
       <c r="K4" s="10">
         <v>-0.3216</v>
@@ -2595,7 +2629,7 @@
         <v>0.4778</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2636,7 +2670,7 @@
         <v>0.16889999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2677,7 +2711,7 @@
         <v>0.54459999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2718,7 +2752,7 @@
         <v>-1.2117</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2759,12 +2793,12 @@
         <v>1.4664999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="13">
-        <v>0.20126666666666662</v>
+        <v>0.20130000000000001</v>
       </c>
       <c r="C9" s="10">
         <v>-0.54890000000000005</v>
@@ -2800,7 +2834,7 @@
         <v>6.0299999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2841,7 +2875,7 @@
         <v>0.31269999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2882,7 +2916,7 @@
         <v>1.1318999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2890,7 +2924,7 @@
         <v>-0.4763</v>
       </c>
       <c r="C12" s="13">
-        <v>-0.45293333333333335</v>
+        <v>-0.45290000000000002</v>
       </c>
       <c r="D12" s="10">
         <v>-0.33360000000000001</v>
@@ -2923,7 +2957,7 @@
         <v>0.23119999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2964,7 +2998,7 @@
         <v>0.20899999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3005,7 +3039,7 @@
         <v>0.55789999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3046,7 +3080,7 @@
         <v>0.29849999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -3093,16 +3127,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3143,7 +3177,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3184,7 +3218,7 @@
         <v>-0.1933</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -3225,7 +3259,7 @@
         <v>-1.3101</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3266,7 +3300,7 @@
         <v>2.5788000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -3283,7 +3317,7 @@
         <v>-6.1600000000000002E-2</v>
       </c>
       <c r="F5" s="12">
-        <v>0.36906666666666671</v>
+        <v>0.36909999999999998</v>
       </c>
       <c r="G5" s="9">
         <v>-0.19980000000000001</v>
@@ -3307,7 +3341,7 @@
         <v>0.76729999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3348,7 +3382,7 @@
         <v>-0.161</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3389,7 +3423,7 @@
         <v>0.22559999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -3430,7 +3464,7 @@
         <v>1.7134</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -3471,7 +3505,7 @@
         <v>-0.28699999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -3512,7 +3546,7 @@
         <v>1.2221</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -3526,7 +3560,7 @@
         <v>0.22919999999999999</v>
       </c>
       <c r="E11" s="12">
-        <v>0.64206666666666667</v>
+        <v>0.6421</v>
       </c>
       <c r="F11" s="9">
         <v>1.1875</v>
@@ -3553,7 +3587,7 @@
         <v>0.2671</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -3594,7 +3628,7 @@
         <v>-0.27239999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -3623,7 +3657,7 @@
         <v>-0.4289</v>
       </c>
       <c r="J13" s="13">
-        <v>-0.10260000000000001</v>
+        <v>-0.1026</v>
       </c>
       <c r="K13" s="9">
         <v>-0.99909999999999999</v>
@@ -3635,7 +3669,7 @@
         <v>0.2162</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -3676,12 +3710,12 @@
         <v>1.0390999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="13">
-        <v>0.4553666666666667</v>
+        <v>0.45540000000000003</v>
       </c>
       <c r="C15" s="9">
         <v>0.56440000000000001</v>
@@ -3717,7 +3751,7 @@
         <v>1.2979000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -3728,7 +3762,7 @@
         <v>-0.22620000000000001</v>
       </c>
       <c r="D16" s="12">
-        <v>-0.34729999999999994</v>
+        <v>-0.3473</v>
       </c>
       <c r="E16" s="8">
         <v>0.40500000000000003</v>
@@ -3740,7 +3774,7 @@
         <v>1.7576000000000001</v>
       </c>
       <c r="H16" s="12">
-        <v>0.84643333333333326</v>
+        <v>0.84640000000000004</v>
       </c>
       <c r="I16" s="9">
         <v>1.3798999999999999</v>
@@ -3755,10 +3789,10 @@
         <v>-1.0851999999999999</v>
       </c>
       <c r="M16" s="12">
-        <v>-1.0799666666666667</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-1.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3773,7 +3807,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3788,7 +3822,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3802,7 +3836,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3817,7 +3851,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3832,7 +3866,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3847,7 +3881,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3861,7 +3895,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3875,7 +3909,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3890,7 +3924,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3905,7 +3939,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3935,16 +3969,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3985,7 +4019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4026,7 +4060,7 @@
         <v>0.19850000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -4067,7 +4101,7 @@
         <v>-1.5982000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4108,7 +4142,7 @@
         <v>1.9187000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -4149,7 +4183,7 @@
         <v>0.95779999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -4190,7 +4224,7 @@
         <v>1.0246</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4231,7 +4265,7 @@
         <v>-0.52849999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -4272,7 +4306,7 @@
         <v>-0.2676</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -4313,7 +4347,7 @@
         <v>0.34039999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -4354,7 +4388,7 @@
         <v>0.45229999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -4380,10 +4414,10 @@
         <v>0.4143</v>
       </c>
       <c r="I11" s="12">
-        <v>-6.6333333333333244E-3</v>
+        <v>-6.6E-3</v>
       </c>
       <c r="J11" s="12">
-        <v>0.15396666666666667</v>
+        <v>0.154</v>
       </c>
       <c r="K11" s="9">
         <v>-0.1119</v>
@@ -4395,7 +4429,7 @@
         <v>0.16170000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -4436,7 +4470,7 @@
         <v>0.20960000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -4477,7 +4511,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -4518,7 +4552,7 @@
         <v>0.97740000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -4559,7 +4593,7 @@
         <v>-1.0412999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -4567,7 +4601,7 @@
         <v>-1.903</v>
       </c>
       <c r="C16" s="12">
-        <v>-0.14446666666666666</v>
+        <v>-0.14449999999999999</v>
       </c>
       <c r="D16" s="9">
         <v>1.5545</v>
@@ -4600,7 +4634,7 @@
         <v>-0.5958</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -4615,7 +4649,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4630,7 +4664,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -4645,7 +4679,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -4660,7 +4694,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4675,7 +4709,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4690,7 +4724,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4705,7 +4739,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4720,7 +4754,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -4735,7 +4769,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4750,7 +4784,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -4780,16 +4814,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4830,7 +4864,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4871,7 +4905,7 @@
         <v>-0.23880000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -4912,7 +4946,7 @@
         <v>-0.87539999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4953,7 +4987,7 @@
         <v>1.0147999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -4994,7 +5028,7 @@
         <v>-0.80569999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -5035,7 +5069,7 @@
         <v>0.89139999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5076,7 +5110,7 @@
         <v>-0.88439999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -5117,7 +5151,7 @@
         <v>0.46439999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -5158,7 +5192,7 @@
         <v>0.57889999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -5199,7 +5233,7 @@
         <v>-0.58509999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -5225,7 +5259,7 @@
         <v>0.15820000000000001</v>
       </c>
       <c r="I11" s="12">
-        <v>0.21316666666666664</v>
+        <v>0.2132</v>
       </c>
       <c r="J11" s="9">
         <v>1.7097</v>
@@ -5234,13 +5268,13 @@
         <v>0.61980000000000002</v>
       </c>
       <c r="L11" s="12">
-        <v>1.16475</v>
+        <v>1.1648000000000001</v>
       </c>
       <c r="M11" s="12">
-        <v>1.16475</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.1648000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -5281,7 +5315,7 @@
         <v>0.52290000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -5322,7 +5356,7 @@
         <v>-0.54159999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -5363,7 +5397,7 @@
         <v>0.14030000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -5404,7 +5438,7 @@
         <v>-2.0924</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -5445,7 +5479,7 @@
         <v>0.84150000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -5460,7 +5494,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5475,7 +5509,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -5490,7 +5524,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -5505,7 +5539,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5520,7 +5554,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -5535,7 +5569,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -5549,7 +5583,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -5564,7 +5598,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -5579,7 +5613,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -5594,7 +5628,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -5624,17 +5658,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -5684,7 +5718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5734,7 +5768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -5784,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5834,7 +5868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5884,7 +5918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5934,7 +5968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -5984,7 +6018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -6034,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6084,7 +6118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6134,7 +6168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -6184,7 +6218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -6234,7 +6268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -6284,7 +6318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -6334,7 +6368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -6384,7 +6418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -6446,19 +6480,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -6508,7 +6542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -6558,7 +6592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -6608,7 +6642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6658,7 +6692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6708,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6758,7 +6792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -6808,7 +6842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -6858,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6908,7 +6942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6958,7 +6992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -7008,7 +7042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -7058,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -7108,7 +7142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -7158,7 +7192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -7208,7 +7242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>1</v>
       </c>

</xml_diff>